<commit_message>
update field and code files
</commit_message>
<xml_diff>
--- a/example-comp/fish-data-comp-species-fields.xlsx
+++ b/example-comp/fish-data-comp-species-fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edlabola\code\fish-data-comp\example-comp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E5D8EA-31E2-4B50-853E-FBBCF6FD3100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E980329F-B094-4798-B5F6-6830A24396DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58A22057-1635-412A-8133-84FB790BB4D0}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="111">
   <si>
     <t>containingTable</t>
   </si>
@@ -92,24 +92,15 @@
     <t>Populations</t>
   </si>
   <si>
-    <t>CommonPopName</t>
-  </si>
-  <si>
     <t>ESU_DPS</t>
   </si>
   <si>
     <t>MajorPopGroup</t>
   </si>
   <si>
-    <t>Population name used by local biologists.</t>
-  </si>
-  <si>
     <t>Text 255</t>
   </si>
   <si>
-    <t>Often this is simply the name of the population(s) as written on the original time series spreadsheets.</t>
-  </si>
-  <si>
     <t>For populations listed under the federal ESA, this is the name of a defined Evolutionarily Significant Unit (ESU) or Distinct Population Segment (DPS) as defined by NMFS Northwest Region or by USFWS.  For non-listed populations this is the DPS or other name.</t>
   </si>
   <si>
@@ -140,12 +131,6 @@
     <t>Partial list: 1 = Chinkook salmon; 2 = Coho salmon; 3 = Steelhead; 4 = Sockeye salmon; 5 = Chum salmon; 6 = Pink salmon; 39 = Mixed salmon; 96 = Mixed anadromous salmonids; 66 = Kokanee; 14 = Bull trout; 10 = Brown trout; 11 = Brook trout; 9 = Rainbow trout; 23 = Redband trout; 111 = Rainbow/redband/steel head trout; 17 = Coastal cutthroat trout; 8 = Cutthroat trout; 94 = Mixed lamprey; 113 = Lamprey (unspecified); 122 = Pacific lamprey; 120 = Western brook lamprey; 15 = Lamprey (CODE DISCONTINUED); 12 = White sturgeon; 44 = Green sturgeon; 98 = N/A; 99 = Unknown</t>
   </si>
   <si>
-    <t>RunID ?</t>
-  </si>
-  <si>
-    <t>LifeHistoryID ?</t>
-  </si>
-  <si>
     <t>FishDist</t>
   </si>
   <si>
@@ -158,9 +143,6 @@
     <t>Code for the fish species.</t>
   </si>
   <si>
-    <t>SubRunID ?</t>
-  </si>
-  <si>
     <t>FishBarrier</t>
   </si>
   <si>
@@ -194,12 +176,6 @@
     <t>If subrun not appropriate for this species, enter 98 = N/A.  Refer to the Trend table for other codes.</t>
   </si>
   <si>
-    <t>PopID from the Coordinated Assessments database.</t>
-  </si>
-  <si>
-    <t>Populate this field to associate this trend with a Coordinated Assessments population, and make this trend available as "related data" in the Coordinated Assessments query system (http://cax.streamnet.org/).</t>
-  </si>
-  <si>
     <t>PTAGIS</t>
   </si>
   <si>
@@ -272,9 +248,6 @@
     <t>hasCodes</t>
   </si>
   <si>
-    <t>PopID ?</t>
-  </si>
-  <si>
     <t>link in 'fieldCodes' is broken. new link is https://www.streamnet.org/resources/nw-fish/fish-species/</t>
   </si>
   <si>
@@ -290,9 +263,6 @@
     <t>sourceDataSystem</t>
   </si>
   <si>
-    <t>Population name(s) used by local biologists.</t>
-  </si>
-  <si>
     <t>Name of "major population group" (MPG) or “stratum” as defined by the NMFS Northwest Region, in which the population falls geographically.</t>
   </si>
   <si>
@@ -395,7 +365,13 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>No?</t>
+    <t>LifeHistoryID</t>
+  </si>
+  <si>
+    <t>RunID</t>
+  </si>
+  <si>
+    <t>SubRunID</t>
   </si>
 </sst>
 </file>
@@ -417,18 +393,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -445,8 +415,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,11 +731,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AE9C97-1A9B-4E5C-B3DE-14E0EEA5BEA2}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H48" sqref="H48"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -780,7 +750,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -798,13 +768,13 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="H1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="I1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -827,13 +797,13 @@
         <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="H2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="I2" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -841,25 +811,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>118</v>
+        <v>92</v>
+      </c>
+      <c r="H3" t="s">
+        <v>107</v>
+      </c>
+      <c r="I3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -870,25 +843,25 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="H4" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="I4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -902,22 +875,22 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="H5" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="I5" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -925,28 +898,28 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="H6" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="I6" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -957,25 +930,22 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="H7" t="s">
-        <v>117</v>
-      </c>
-      <c r="I7" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -989,19 +959,22 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="H8" t="s">
-        <v>117</v>
+        <v>107</v>
+      </c>
+      <c r="I8" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1009,28 +982,28 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="H9" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="I9" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1038,25 +1011,25 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G10" t="s">
-        <v>103</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>118</v>
+        <v>94</v>
+      </c>
+      <c r="H10" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1067,25 +1040,25 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="H11" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="I11" t="s">
-        <v>78</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1093,25 +1066,28 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="G12" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="H12" t="s">
-        <v>117</v>
+        <v>107</v>
+      </c>
+      <c r="I12" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1119,28 +1095,25 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
         <v>19</v>
       </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G13" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="H13" t="s">
-        <v>117</v>
-      </c>
-      <c r="I13" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1148,25 +1121,28 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
         <v>21</v>
-      </c>
-      <c r="E14" t="s">
-        <v>20</v>
       </c>
       <c r="F14" t="s">
         <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>104</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>118</v>
+        <v>95</v>
+      </c>
+      <c r="H14" t="s">
+        <v>107</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1174,7 +1150,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -1189,13 +1165,13 @@
         <v>9</v>
       </c>
       <c r="G15" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="H15" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="I15" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1203,25 +1179,25 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
         <v>23</v>
       </c>
-      <c r="F16" t="s">
-        <v>26</v>
-      </c>
       <c r="G16" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="H16" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1229,28 +1205,28 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
         <v>19</v>
       </c>
-      <c r="D17" t="s">
-        <v>21</v>
-      </c>
       <c r="E17" t="s">
+        <v>74</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" t="s">
+        <v>107</v>
+      </c>
+      <c r="I17" t="s">
         <v>24</v>
-      </c>
-      <c r="F17" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" t="s">
-        <v>105</v>
-      </c>
-      <c r="H17" t="s">
-        <v>117</v>
-      </c>
-      <c r="I17" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1258,25 +1234,28 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="G18" t="s">
-        <v>105</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>118</v>
+        <v>97</v>
+      </c>
+      <c r="H18" t="s">
+        <v>107</v>
+      </c>
+      <c r="I18" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1284,28 +1263,25 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="F19" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G19" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="H19" t="s">
-        <v>117</v>
-      </c>
-      <c r="I19" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1313,450 +1289,459 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
       </c>
       <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
         <v>21</v>
       </c>
-      <c r="E20" t="s">
-        <v>23</v>
-      </c>
       <c r="F20" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G20" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="H20" t="s">
-        <v>117</v>
+        <v>107</v>
+      </c>
+      <c r="I20" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>84</v>
+        <v>28</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G21" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H21" t="s">
-        <v>117</v>
-      </c>
-      <c r="I21" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>108</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E22" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="G22" t="s">
-        <v>106</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>118</v>
+        <v>98</v>
+      </c>
+      <c r="H22" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="F23" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="G23" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H23" t="s">
-        <v>117</v>
-      </c>
-      <c r="I23" t="s">
-        <v>78</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>109</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E24" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="F24" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="G24" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H24" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>110</v>
       </c>
       <c r="D25" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="F25" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="G25" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H25" t="s">
-        <v>117</v>
-      </c>
-      <c r="I25" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E26" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="F26" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="G26" t="s">
-        <v>107</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>118</v>
+        <v>100</v>
+      </c>
+      <c r="H26" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E27" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F27" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G27" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="H27" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E28" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="F28" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="G28" t="s">
-        <v>108</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>118</v>
+        <v>100</v>
+      </c>
+      <c r="H28" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="F29" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="G29" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="H29" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>36</v>
+        <v>81</v>
       </c>
       <c r="D30" t="s">
-        <v>30</v>
+        <v>89</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="F30" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="G30" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="H30" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>33</v>
+        <v>103</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="E31" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="F31" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="G31" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="H31" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D32" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="E32" t="s">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="F32" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="G32" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="H32" t="s">
-        <v>117</v>
+        <v>107</v>
+      </c>
+      <c r="I32" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D33" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="E33" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="F33" t="s">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="G33" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="H33" t="s">
-        <v>117</v>
+        <v>107</v>
+      </c>
+      <c r="I33" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D34" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="E34" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="F34" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="G34" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="H34" t="s">
-        <v>117</v>
+        <v>107</v>
+      </c>
+      <c r="I34" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C35" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="D35" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="E35" t="s">
-        <v>46</v>
+        <v>78</v>
       </c>
       <c r="F35" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="G35" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="H35" t="s">
-        <v>117</v>
+        <v>107</v>
+      </c>
+      <c r="I35" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="D36" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F36" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="G36" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="H36" t="s">
-        <v>117</v>
+        <v>107</v>
+      </c>
+      <c r="I36" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -1764,25 +1749,31 @@
         <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>91</v>
-      </c>
-      <c r="D37" t="s">
-        <v>99</v>
+        <v>55</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="E37" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="F37" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="G37" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="H37" t="s">
-        <v>117</v>
+        <v>107</v>
+      </c>
+      <c r="I37" t="s">
+        <v>61</v>
+      </c>
+      <c r="J37" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -1790,25 +1781,31 @@
         <v>53</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" t="s">
-        <v>99</v>
+        <v>55</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="E38" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="F38" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="G38" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="H38" t="s">
-        <v>117</v>
+        <v>107</v>
+      </c>
+      <c r="I38" t="s">
+        <v>63</v>
+      </c>
+      <c r="J38" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
@@ -1816,28 +1813,31 @@
         <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C39" t="s">
         <v>55</v>
       </c>
-      <c r="D39" t="s">
-        <v>98</v>
+      <c r="D39" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="E39" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="F39" t="s">
+        <v>60</v>
+      </c>
+      <c r="G39" t="s">
         <v>90</v>
       </c>
-      <c r="G39" t="s">
-        <v>85</v>
-      </c>
       <c r="H39" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="I39" t="s">
-        <v>111</v>
+        <v>65</v>
+      </c>
+      <c r="J39" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
@@ -1845,244 +1845,32 @@
         <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
-      </c>
-      <c r="D40" t="s">
-        <v>98</v>
+        <v>55</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="E40" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="F40" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="G40" t="s">
-        <v>85</v>
-      </c>
-      <c r="H40" t="s">
-        <v>117</v>
-      </c>
-      <c r="I40" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" t="s">
-        <v>56</v>
-      </c>
-      <c r="D41" t="s">
-        <v>98</v>
-      </c>
-      <c r="E41" t="s">
-        <v>88</v>
-      </c>
-      <c r="F41" t="s">
-        <v>89</v>
-      </c>
-      <c r="G41" t="s">
-        <v>85</v>
-      </c>
-      <c r="H41" t="s">
-        <v>117</v>
-      </c>
-      <c r="I41" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>53</v>
-      </c>
-      <c r="B42" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" t="s">
-        <v>56</v>
-      </c>
-      <c r="D42" t="s">
-        <v>98</v>
-      </c>
-      <c r="E42" t="s">
-        <v>88</v>
-      </c>
-      <c r="F42" t="s">
-        <v>89</v>
-      </c>
-      <c r="G42" t="s">
-        <v>85</v>
-      </c>
-      <c r="H42" t="s">
-        <v>117</v>
-      </c>
-      <c r="I42" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43" t="s">
-        <v>60</v>
-      </c>
-      <c r="C43" t="s">
-        <v>56</v>
-      </c>
-      <c r="D43" t="s">
-        <v>98</v>
-      </c>
-      <c r="E43" t="s">
-        <v>88</v>
-      </c>
-      <c r="F43" t="s">
-        <v>89</v>
-      </c>
-      <c r="G43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H43" t="s">
-        <v>117</v>
-      </c>
-      <c r="I43" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E44" t="s">
-        <v>67</v>
-      </c>
-      <c r="F44" t="s">
-        <v>68</v>
-      </c>
-      <c r="G44" t="s">
-        <v>100</v>
-      </c>
-      <c r="H44" t="s">
-        <v>117</v>
-      </c>
-      <c r="I44" t="s">
-        <v>69</v>
-      </c>
-      <c r="J44" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>61</v>
-      </c>
-      <c r="B45" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" t="s">
-        <v>63</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E45" t="s">
-        <v>70</v>
-      </c>
-      <c r="F45" t="s">
-        <v>68</v>
-      </c>
-      <c r="G45" t="s">
-        <v>100</v>
-      </c>
-      <c r="H45" t="s">
-        <v>117</v>
-      </c>
-      <c r="I45" t="s">
-        <v>71</v>
-      </c>
-      <c r="J45" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>61</v>
-      </c>
-      <c r="B46" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E46" t="s">
-        <v>72</v>
-      </c>
-      <c r="F46" t="s">
-        <v>68</v>
-      </c>
-      <c r="G46" t="s">
-        <v>100</v>
-      </c>
-      <c r="H46" t="s">
-        <v>117</v>
-      </c>
-      <c r="I46" t="s">
-        <v>73</v>
-      </c>
-      <c r="J46" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>61</v>
-      </c>
-      <c r="B47" t="s">
-        <v>66</v>
-      </c>
-      <c r="C47" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E47" t="s">
-        <v>81</v>
-      </c>
-      <c r="F47" t="s">
-        <v>81</v>
-      </c>
-      <c r="G47" t="s">
-        <v>100</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="I47" s="1" t="s">
-        <v>115</v>
+        <v>90</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I47" xr:uid="{A6AE9C97-1A9B-4E5C-B3DE-14E0EEA5BEA2}"/>
+  <autoFilter ref="A1:I40" xr:uid="{A6AE9C97-1A9B-4E5C-B3DE-14E0EEA5BEA2}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update files and add csv version
</commit_message>
<xml_diff>
--- a/example-comp/fish-data-comp-species-fields.xlsx
+++ b/example-comp/fish-data-comp-species-fields.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edlabola\code\fish-data-comp\example-comp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edlabola\OneDrive - DOI\StreamNetFAIRAssessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E980329F-B094-4798-B5F6-6830A24396DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCB7F63-7778-4387-856E-410F8FF98ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58A22057-1635-412A-8133-84FB790BB4D0}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="112">
   <si>
     <t>containingTable</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Common name of the taxon of fish.</t>
   </si>
   <si>
-    <t>Enter the name of the taxon here, even if taxon name is included in the name of the population. Select from the following: Bull Trout; Chinook salmon; Chum salmon; Coho salmon; Sockeye salmon; Steelhead; Additional species may be added in the future: refer to http://old.streamnet.org/SpeciesInFW.html for common names.</t>
-  </si>
-  <si>
     <t>RperS</t>
   </si>
   <si>
@@ -101,18 +98,6 @@
     <t>Text 255</t>
   </si>
   <si>
-    <t>For populations listed under the federal ESA, this is the name of a defined Evolutionarily Significant Unit (ESU) or Distinct Population Segment (DPS) as defined by NMFS Northwest Region or by USFWS.  For non-listed populations this is the DPS or other name.</t>
-  </si>
-  <si>
-    <t>Name of "major population group" (MPG) or “stratum” as defined by the NMFS Northwest Region, in which the population falls.</t>
-  </si>
-  <si>
-    <t>The term "stratum" is used in the Willamette/Lower Columbia Recovery Domain, while "major population group" is used in other areas.  The term "stratum" includes life history considerations as well as geographic criteria, while MPGs are defined geographically.  See Appendix C for the list of MPGs / strata.</t>
-  </si>
-  <si>
-    <t>Enter the name of the ESU or DPS here.  Entries in this field are taxonomic divisions defined by NMFS or USFWS, and may be at the species, subspecies, or finer scale.  ESUs of salmon north of California are listed at https://web.archive.org/web/*/http://www.nwfsc.noaa.gov/trt/.</t>
-  </si>
-  <si>
     <t>Appendix C is 'ca-populations' file.</t>
   </si>
   <si>
@@ -149,18 +134,12 @@
     <t>Code for the fish species blocked by the barrier.</t>
   </si>
   <si>
-    <t>Refer to Trend table information.  Create records in this table only for specific taxa.  That is, do not use codes such as 55 ("Miscellaneous freshwater species"), 93 ("Not specified"), 98("N/A"), 99 ("Unknown"), or 125 ("Other").</t>
-  </si>
-  <si>
     <t>Byte</t>
   </si>
   <si>
     <t>Code for the fish run blocked by the barrier.</t>
   </si>
   <si>
-    <t>If run not appropriate for this species, enter 98 = N/A.  Refer to the Trend table for other codes.</t>
-  </si>
-  <si>
     <t>Code for the life history strategy(s) of the species in the indicated reach.</t>
   </si>
   <si>
@@ -173,9 +152,6 @@
     <t>Code for the fish subrun.</t>
   </si>
   <si>
-    <t>If subrun not appropriate for this species, enter 98 = N/A.  Refer to the Trend table for other codes.</t>
-  </si>
-  <si>
     <t>PTAGIS</t>
   </si>
   <si>
@@ -230,15 +206,9 @@
     <t>Code indicating species of this recovered fish</t>
   </si>
   <si>
-    <t>Max cols = 2; Required; Lookcup; Must match the value in corresponding Catch/Sample data file, species</t>
-  </si>
-  <si>
     <t>Code indicating species of this catch group</t>
   </si>
   <si>
-    <t>Max cols = 2; Required; Lookcup; Must match the value in corresponding Reocvery data file, species</t>
-  </si>
-  <si>
     <t>codes same as 1989 data standard + 9 is atlantic salmon</t>
   </si>
   <si>
@@ -263,9 +233,6 @@
     <t>sourceDataSystem</t>
   </si>
   <si>
-    <t>Name of "major population group" (MPG) or “stratum” as defined by the NMFS Northwest Region, in which the population falls geographically.</t>
-  </si>
-  <si>
     <t>Data Specifications / Validation Codes / SRR Codes</t>
   </si>
   <si>
@@ -275,9 +242,6 @@
     <t>A 1-character code representing the species of the fish being sampled. Must be used with run and rear type codes to create the whole SRR code.</t>
   </si>
   <si>
-    <t>Three-character code that identifies the species, run, and rear type of fish. The first character represents the species, the second character represents the run, and the third character represents the rearing type.</t>
-  </si>
-  <si>
     <t>SRR Verbose Validation Codes from https://www.ptagis.org/Resources/ValidationCodes?domainFilter=SrrCode</t>
   </si>
   <si>
@@ -372,6 +336,45 @@
   </si>
   <si>
     <t>SubRunID</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>Enter the name of the taxon here even if taxon name is included in the name of the population. Select from the following: Bull Trout; Chinook salmon; Chum salmon; Coho salmon; Sockeye salmon; Steelhead; Additional species may be added in the future: refer to http://old.streamnet.org/SpeciesInFW.html for common names.</t>
+  </si>
+  <si>
+    <t>Name of "major population group" (MPG) or “stratum” as defined by the NMFS Northwest Region in which the population falls.</t>
+  </si>
+  <si>
+    <t>Name of "major population group" (MPG) or “stratum” as defined by the NMFS Northwest Region in which the population falls geographically.</t>
+  </si>
+  <si>
+    <t>If run not appropriate for this species enter 98 = N/A.  Refer to the Trend table for other codes.</t>
+  </si>
+  <si>
+    <t>Refer to Trend table information.  Create records in this table only for specific taxa.  That is do not use codes such as 55 ("Miscellaneous freshwater species") 93 ("Not specified") 98("N/A") 99 ("Unknown")or 125 ("Other").</t>
+  </si>
+  <si>
+    <t>Three-character code that identifies the species run and rear type of fish. The first character represents the species the second character represents the run and the third character represents the rearing type.</t>
+  </si>
+  <si>
+    <t>Max cols = 2; Required; Lookcup; Must match the value in corresponding Catch/Sample data file species</t>
+  </si>
+  <si>
+    <t>Max cols = 2; Required; Lookcup; Must match the value in corresponding Reocvery data file species</t>
+  </si>
+  <si>
+    <t>For populations listed under the federal ESA this is the name of a defined Evolutionarily Significant Unit (ESU) or Distinct Population Segment (DPS) as defined by NMFS Northwest Region or by USFWS.  For non-listed populations this is the DPS or other name.</t>
+  </si>
+  <si>
+    <t>If subrun not appropriate for this species enter 98 = N/A.  Refer to the Trend table for other codes.</t>
+  </si>
+  <si>
+    <t>Enter the name of the ESU or DPS here.  Entries in this field are taxonomic divisions defined by NMFS or USFWS and may be at the species subspecies or finer scale.  ESUs of salmon north of California are listed at https://web.archive.org/web/*/http://www.nwfsc.noaa.gov/trt/.</t>
+  </si>
+  <si>
+    <t>The term "stratum" is used in the Willamette/Lower Columbia Recovery Domain while "major population group" is used in other areas.  The term "stratum" includes life history considerations as well as geographic criteria while MPGs are defined geographically.  See Appendix C for the list of MPGs / strata.</t>
   </si>
 </sst>
 </file>
@@ -735,7 +738,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -750,7 +753,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -768,13 +771,13 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="H1" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="I1" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -782,7 +785,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -794,16 +797,16 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="H2" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -811,7 +814,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -823,16 +826,16 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -840,28 +843,28 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="G4" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="H4" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I4" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -869,28 +872,28 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I5" t="s">
         <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>92</v>
-      </c>
-      <c r="H5" t="s">
-        <v>107</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -898,7 +901,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -910,16 +913,16 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="G6" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="H6" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I6" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -927,25 +930,28 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="G7" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="H7" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="I7" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -953,28 +959,28 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>18</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" t="s">
         <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H8" t="s">
-        <v>107</v>
-      </c>
-      <c r="I8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -982,7 +988,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -994,16 +1000,16 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="H9" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1011,25 +1017,28 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="H10" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="I10" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1037,28 +1046,28 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
         <v>18</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I11" t="s">
         <v>19</v>
-      </c>
-      <c r="E11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" t="s">
-        <v>94</v>
-      </c>
-      <c r="H11" t="s">
-        <v>107</v>
-      </c>
-      <c r="I11" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1066,7 +1075,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
@@ -1078,16 +1087,16 @@
         <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="G12" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="H12" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I12" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1095,25 +1104,28 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="F13" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="G13" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="H13" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="I13" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1121,28 +1133,28 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
         <v>18</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" t="s">
+        <v>111</v>
+      </c>
+      <c r="G14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" t="s">
+        <v>95</v>
+      </c>
+      <c r="I14" t="s">
         <v>19</v>
-      </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H14" t="s">
-        <v>107</v>
-      </c>
-      <c r="I14" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1150,7 +1162,7 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
@@ -1162,16 +1174,16 @@
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="G15" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="H15" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I15" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1179,25 +1191,28 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="F16" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="G16" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="H16" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="I16" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1205,28 +1220,28 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" t="s">
         <v>18</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F17" t="s">
+        <v>111</v>
+      </c>
+      <c r="G17" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" t="s">
+        <v>95</v>
+      </c>
+      <c r="I17" t="s">
         <v>19</v>
-      </c>
-      <c r="E17" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" t="s">
-        <v>96</v>
-      </c>
-      <c r="H17" t="s">
-        <v>107</v>
-      </c>
-      <c r="I17" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1234,7 +1249,7 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
@@ -1246,16 +1261,16 @@
         <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="H18" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I18" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1263,25 +1278,28 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
         <v>16</v>
       </c>
-      <c r="C19" t="s">
-        <v>17</v>
-      </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>108</v>
       </c>
       <c r="F19" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="G19" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="H19" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="I19" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1289,584 +1307,617 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" t="s">
         <v>18</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" t="s">
+        <v>111</v>
+      </c>
+      <c r="G20" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" t="s">
+        <v>95</v>
+      </c>
+      <c r="I20" t="s">
         <v>19</v>
-      </c>
-      <c r="E20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G20" t="s">
-        <v>97</v>
-      </c>
-      <c r="H20" t="s">
-        <v>107</v>
-      </c>
-      <c r="I20" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
         <v>26</v>
       </c>
-      <c r="C21" t="s">
-        <v>31</v>
-      </c>
       <c r="D21" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E21" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F21" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G21" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="H21" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="I21" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F22" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G22" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="H22" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="I22" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
         <v>25</v>
       </c>
-      <c r="B23" t="s">
-        <v>30</v>
-      </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" t="s">
         <v>27</v>
       </c>
-      <c r="E23" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" t="s">
-        <v>32</v>
-      </c>
       <c r="G23" t="s">
+        <v>87</v>
+      </c>
+      <c r="H23" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" t="s">
         <v>99</v>
-      </c>
-      <c r="H23" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
         <v>25</v>
       </c>
-      <c r="B24" t="s">
-        <v>30</v>
-      </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F24" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="G24" t="s">
+        <v>87</v>
+      </c>
+      <c r="H24" t="s">
+        <v>95</v>
+      </c>
+      <c r="I24" t="s">
         <v>99</v>
-      </c>
-      <c r="H24" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" t="s">
         <v>25</v>
       </c>
-      <c r="B25" t="s">
-        <v>30</v>
-      </c>
       <c r="C25" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F25" t="s">
-        <v>44</v>
+        <v>109</v>
       </c>
       <c r="G25" t="s">
+        <v>87</v>
+      </c>
+      <c r="H25" t="s">
+        <v>95</v>
+      </c>
+      <c r="I25" t="s">
         <v>99</v>
-      </c>
-      <c r="H25" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E26" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F26" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="G26" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H26" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="I26" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>39</v>
+        <v>103</v>
       </c>
       <c r="G27" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H27" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="I27" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" t="s">
         <v>34</v>
       </c>
-      <c r="C28" t="s">
-        <v>108</v>
-      </c>
-      <c r="D28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" t="s">
-        <v>41</v>
-      </c>
       <c r="G28" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="H28" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="I28" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D29" t="s">
         <v>76</v>
       </c>
-      <c r="D29" t="s">
-        <v>88</v>
-      </c>
       <c r="E29" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F29" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="G29" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H29" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="I29" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D30" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="E30" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="F30" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="G30" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H30" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="I30" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="E31" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="F31" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="G31" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H31" t="s">
-        <v>107</v>
+        <v>95</v>
+      </c>
+      <c r="I31" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C32" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E32" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="F32" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="G32" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H32" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I32" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="F33" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="G33" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H33" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I33" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E34" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="F34" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="G34" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H34" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I34" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E35" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="F35" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="G35" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H35" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I35" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D36" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E36" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="F36" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="G36" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="H36" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="I36" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" t="s">
+        <v>52</v>
+      </c>
+      <c r="G37" t="s">
+        <v>78</v>
+      </c>
+      <c r="H37" t="s">
+        <v>95</v>
+      </c>
+      <c r="I37" t="s">
         <v>53</v>
       </c>
-      <c r="B37" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E37" t="s">
-        <v>59</v>
-      </c>
-      <c r="F37" t="s">
-        <v>60</v>
-      </c>
-      <c r="G37" t="s">
-        <v>90</v>
-      </c>
-      <c r="H37" t="s">
-        <v>107</v>
-      </c>
-      <c r="I37" t="s">
-        <v>61</v>
-      </c>
       <c r="J37" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" t="s">
+        <v>52</v>
+      </c>
+      <c r="G38" t="s">
+        <v>78</v>
+      </c>
+      <c r="H38" t="s">
+        <v>95</v>
+      </c>
+      <c r="I38" t="s">
+        <v>106</v>
+      </c>
+      <c r="J38" t="s">
         <v>56</v>
-      </c>
-      <c r="C38" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E38" t="s">
-        <v>62</v>
-      </c>
-      <c r="F38" t="s">
-        <v>60</v>
-      </c>
-      <c r="G38" t="s">
-        <v>90</v>
-      </c>
-      <c r="H38" t="s">
-        <v>107</v>
-      </c>
-      <c r="I38" t="s">
-        <v>63</v>
-      </c>
-      <c r="J38" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" t="s">
         <v>55</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" t="s">
-        <v>64</v>
-      </c>
       <c r="F39" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G39" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H39" t="s">
+        <v>95</v>
+      </c>
+      <c r="I39" t="s">
         <v>107</v>
       </c>
-      <c r="I39" t="s">
-        <v>65</v>
-      </c>
       <c r="J39" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E40" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F40" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="G40" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update comp, add xwalk and templates
</commit_message>
<xml_diff>
--- a/example-comp/fish-data-comp-species-fields.xlsx
+++ b/example-comp/fish-data-comp-species-fields.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edlabola\OneDrive - DOI\StreamNetFAIRAssessment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edlabola\code\fish-data-comp\example-comp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCB7F63-7778-4387-856E-410F8FF98ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C1AEA5-712F-4249-90A8-7F6266FE4A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58A22057-1635-412A-8133-84FB790BB4D0}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="134">
   <si>
     <t>containingTable</t>
   </si>
@@ -375,6 +375,72 @@
   </si>
   <si>
     <t>The term "stratum" is used in the Willamette/Lower Columbia Recovery Domain while "major population group" is used in other areas.  The term "stratum" includes life history considerations as well as geographic criteria while MPGs are defined geographically.  See Appendix C for the list of MPGs / strata.</t>
+  </si>
+  <si>
+    <t>RearingType</t>
+  </si>
+  <si>
+    <t>The rearing type (origin; production type) of the fish represented by this record.</t>
+  </si>
+  <si>
+    <t>Text 8</t>
+  </si>
+  <si>
+    <t>Acceptable values include Natural; Mixed; Unknown</t>
+  </si>
+  <si>
+    <t>ProdID</t>
+  </si>
+  <si>
+    <t>Code for the production type of the fish.  For redd counts indicate the production type(s) of the fish that created the redds.</t>
+  </si>
+  <si>
+    <t>StreamNet-DataExchangeStandard20200204 B1</t>
+  </si>
+  <si>
+    <t>1 = Hatchery; 2 = Natural; 3 = Mixed; 99 = Unknown</t>
+  </si>
+  <si>
+    <t>Sampled Run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code to indicate run when sample is stratified by entry run timing (e.g. freshwater sport fisheries where runs can be sampled_run identified by morphological differences); </t>
+  </si>
+  <si>
+    <t>If present must match one of the following: 1= Spring; 2 = Summer; 3 = Fall (includes type S Coho); 4 = Winter; 5 = Hybrid; 6 = Landlocked; 7 = Late Fall (includes N type Coho); 8 = Late Fall Upriver Bright Chinook. Must match the value listed in corresponding Catch/Sample data file, sample_run</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Code to indicate run of this release group</t>
+  </si>
+  <si>
+    <t>Code to indicate run when sample is stratified by entry run timing (e.g. freshwater sport fisheries where runs can be sampled_run identified by morphological differences)</t>
+  </si>
+  <si>
+    <t>If present must match one of the following: 1= Spring; 2 = Summer; 3 = Fall (includes type S Coho); 4 = Winter; 5 = Hybrid; 6 = Landlocked; 7 = Late Fall (includes N type Coho); 8 = Late Fall Upriver Bright Chinook; 9 = Late Winter. Must match the value listed in corresponding Catch/Sample data file, sample_run. Must match the value in corresponding Recovery data file, sampled_run</t>
+  </si>
+  <si>
+    <t>If present must match one of the following: 1= Spring; 2 = Summer; 3 = Fall (includes type S Coho); 4 = Winter; 5 = Hybrid; 6 = Landlocked; 7 = Late Fall (includes N type Coho); 8 = Late Fall Upriver Bright Chinook</t>
+  </si>
+  <si>
+    <t>Rearing Type</t>
+  </si>
+  <si>
+    <t>Code indicating most prevalent rearing method for this release group</t>
+  </si>
+  <si>
+    <t>If present, must match one of the following: H = Hatchery reared fish (includes any portion of fish’s life history in hatchery or artificially enhanced environment); W = Wild fish; M = mixed hatchery  &amp; wild (downstream migrant or marine tagging); U = Unknown (unavailable from release agency)</t>
+  </si>
+  <si>
+    <t>Text 20</t>
+  </si>
+  <si>
+    <t>Select from the following: Spring; Summer; Fall; Late fall; Winter; Spring/summer; Both summer &amp; winter; Early; Late; Both early &amp; late; N/A (for species without recognized runs)</t>
+  </si>
+  <si>
+    <t>Enter the name of the run here even if  run name is included in the name of the population. Entries in this field are not recognized as taxonomic divisions</t>
   </si>
 </sst>
 </file>
@@ -416,10 +482,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -734,11 +801,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AE9C97-1A9B-4E5C-B3DE-14E0EEA5BEA2}">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -814,28 +881,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>100</v>
+        <v>131</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="G3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H3" t="s">
         <v>95</v>
       </c>
       <c r="I3" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -846,16 +913,16 @@
         <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G4" t="s">
         <v>80</v>
@@ -864,7 +931,7 @@
         <v>95</v>
       </c>
       <c r="I4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -875,16 +942,16 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>123</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F5" t="s">
-        <v>111</v>
+        <v>131</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="G5" t="s">
         <v>80</v>
@@ -893,7 +960,7 @@
         <v>95</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -901,28 +968,28 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="F6" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="G6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H6" t="s">
         <v>95</v>
       </c>
       <c r="I6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -930,28 +997,28 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="F7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H7" t="s">
         <v>95</v>
       </c>
       <c r="I7" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -959,28 +1026,28 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>114</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="F8" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="G8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H8" t="s">
         <v>95</v>
       </c>
       <c r="I8" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -988,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
         <v>3</v>
@@ -1003,7 +1070,7 @@
         <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H9" t="s">
         <v>95</v>
@@ -1017,22 +1084,22 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>123</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" t="s">
-        <v>108</v>
-      </c>
-      <c r="F10" t="s">
-        <v>110</v>
+        <v>131</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="G10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H10" t="s">
         <v>95</v>
@@ -1046,28 +1113,28 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="F11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H11" t="s">
         <v>95</v>
       </c>
       <c r="I11" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1075,28 +1142,28 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="F12" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="G12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H12" t="s">
         <v>95</v>
       </c>
       <c r="I12" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1104,28 +1171,28 @@
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>108</v>
+        <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H13" t="s">
         <v>95</v>
       </c>
       <c r="I13" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1133,28 +1200,28 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>123</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" t="s">
-        <v>101</v>
-      </c>
-      <c r="F14" t="s">
-        <v>111</v>
+        <v>131</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="G14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H14" t="s">
         <v>95</v>
       </c>
       <c r="I14" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1162,28 +1229,28 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>108</v>
       </c>
       <c r="F15" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="G15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H15" t="s">
         <v>95</v>
       </c>
       <c r="I15" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1191,28 +1258,28 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="F16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H16" t="s">
         <v>95</v>
       </c>
       <c r="I16" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1220,28 +1287,28 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="G17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H17" t="s">
         <v>95</v>
       </c>
       <c r="I17" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1249,28 +1316,28 @@
         <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" t="s">
-        <v>100</v>
+        <v>131</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="G18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H18" t="s">
         <v>95</v>
       </c>
       <c r="I18" t="s">
-        <v>59</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1278,7 +1345,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
         <v>16</v>
@@ -1293,7 +1360,7 @@
         <v>110</v>
       </c>
       <c r="G19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H19" t="s">
         <v>95</v>
@@ -1307,7 +1374,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -1322,7 +1389,7 @@
         <v>111</v>
       </c>
       <c r="G20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H20" t="s">
         <v>95</v>
@@ -1333,54 +1400,54 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D21" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="G21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H21" t="s">
         <v>95</v>
       </c>
       <c r="I21" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" t="s">
-        <v>33</v>
-      </c>
-      <c r="F22" t="s">
-        <v>34</v>
+        <v>131</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="G22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H22" t="s">
         <v>95</v>
@@ -1391,25 +1458,25 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C23" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E23" t="s">
-        <v>28</v>
+        <v>108</v>
       </c>
       <c r="F23" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="G23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H23" t="s">
         <v>95</v>
@@ -1420,83 +1487,83 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>97</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>35</v>
+        <v>102</v>
       </c>
       <c r="F24" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="G24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H24" t="s">
         <v>95</v>
       </c>
       <c r="I24" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>98</v>
+        <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="G25" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H25" t="s">
         <v>95</v>
       </c>
       <c r="I25" t="s">
-        <v>99</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>123</v>
       </c>
       <c r="D26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E26" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" t="s">
-        <v>104</v>
+        <v>131</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="G26" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H26" t="s">
         <v>95</v>
@@ -1507,25 +1574,25 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>97</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E27" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="F27" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="G27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H27" t="s">
         <v>95</v>
@@ -1536,54 +1603,54 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="E28" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="F28" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="G28" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H28" t="s">
         <v>95</v>
       </c>
       <c r="I28" t="s">
-        <v>99</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="E29" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="F29" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="G29" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="H29" t="s">
         <v>95</v>
@@ -1594,25 +1661,25 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>31</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="F30" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="G30" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="H30" t="s">
         <v>95</v>
@@ -1623,25 +1690,25 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>26</v>
       </c>
       <c r="D31" t="s">
-        <v>77</v>
+        <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>71</v>
+        <v>28</v>
       </c>
       <c r="F31" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="G31" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="H31" t="s">
         <v>95</v>
@@ -1652,276 +1719,653 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>105</v>
+        <v>35</v>
       </c>
       <c r="F32" t="s">
-        <v>68</v>
+        <v>103</v>
       </c>
       <c r="G32" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="H32" t="s">
         <v>95</v>
       </c>
       <c r="I32" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="E33" t="s">
-        <v>105</v>
+        <v>36</v>
       </c>
       <c r="F33" t="s">
-        <v>67</v>
+        <v>109</v>
       </c>
       <c r="G33" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="H33" t="s">
         <v>95</v>
       </c>
       <c r="I33" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C34" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="E34" t="s">
-        <v>105</v>
+        <v>30</v>
       </c>
       <c r="F34" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="G34" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="H34" t="s">
         <v>95</v>
       </c>
       <c r="I34" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="D35" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="E35" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="F35" t="s">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="G35" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="H35" t="s">
         <v>95</v>
       </c>
       <c r="I35" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="D36" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="E36" t="s">
-        <v>105</v>
+        <v>33</v>
       </c>
       <c r="F36" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="G36" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="H36" t="s">
         <v>95</v>
       </c>
       <c r="I36" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>77</v>
+        <v>116</v>
+      </c>
+      <c r="D37" t="s">
+        <v>31</v>
       </c>
       <c r="E37" t="s">
-        <v>51</v>
+        <v>117</v>
       </c>
       <c r="F37" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="G37" t="s">
-        <v>78</v>
+        <v>118</v>
       </c>
       <c r="H37" t="s">
         <v>95</v>
       </c>
       <c r="I37" t="s">
-        <v>53</v>
-      </c>
-      <c r="J37" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="C38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>77</v>
+        <v>65</v>
+      </c>
+      <c r="D38" t="s">
+        <v>76</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="F38" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="G38" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="H38" t="s">
         <v>95</v>
       </c>
       <c r="I38" t="s">
-        <v>106</v>
-      </c>
-      <c r="J38" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="C39" t="s">
-        <v>47</v>
-      </c>
-      <c r="D39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" t="s">
         <v>77</v>
       </c>
       <c r="E39" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="F39" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="G39" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="H39" t="s">
         <v>95</v>
       </c>
       <c r="I39" t="s">
-        <v>107</v>
-      </c>
-      <c r="J39" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" t="s">
+        <v>71</v>
+      </c>
+      <c r="F40" t="s">
+        <v>74</v>
+      </c>
+      <c r="G40" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40" t="s">
+        <v>95</v>
+      </c>
+      <c r="I40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" t="s">
+        <v>76</v>
+      </c>
+      <c r="E41" t="s">
+        <v>105</v>
+      </c>
+      <c r="F41" t="s">
+        <v>68</v>
+      </c>
+      <c r="G41" t="s">
+        <v>64</v>
+      </c>
+      <c r="H41" t="s">
+        <v>95</v>
+      </c>
+      <c r="I41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" t="s">
+        <v>76</v>
+      </c>
+      <c r="E42" t="s">
+        <v>105</v>
+      </c>
+      <c r="F42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G42" t="s">
+        <v>64</v>
+      </c>
+      <c r="H42" t="s">
+        <v>95</v>
+      </c>
+      <c r="I42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" t="s">
+        <v>40</v>
+      </c>
+      <c r="D43" t="s">
+        <v>76</v>
+      </c>
+      <c r="E43" t="s">
+        <v>105</v>
+      </c>
+      <c r="F43" t="s">
+        <v>67</v>
+      </c>
+      <c r="G43" t="s">
+        <v>64</v>
+      </c>
+      <c r="H43" t="s">
+        <v>95</v>
+      </c>
+      <c r="I43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D44" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44" t="s">
+        <v>105</v>
+      </c>
+      <c r="F44" t="s">
+        <v>67</v>
+      </c>
+      <c r="G44" t="s">
+        <v>64</v>
+      </c>
+      <c r="H44" t="s">
+        <v>95</v>
+      </c>
+      <c r="I44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" t="s">
+        <v>40</v>
+      </c>
+      <c r="D45" t="s">
+        <v>76</v>
+      </c>
+      <c r="E45" t="s">
+        <v>105</v>
+      </c>
+      <c r="F45" t="s">
+        <v>67</v>
+      </c>
+      <c r="G45" t="s">
+        <v>64</v>
+      </c>
+      <c r="H45" t="s">
+        <v>95</v>
+      </c>
+      <c r="I45" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>45</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E46" t="s">
+        <v>51</v>
+      </c>
+      <c r="F46" t="s">
+        <v>52</v>
+      </c>
+      <c r="G46" t="s">
+        <v>78</v>
+      </c>
+      <c r="H46" t="s">
+        <v>95</v>
+      </c>
+      <c r="I46" t="s">
+        <v>53</v>
+      </c>
+      <c r="J46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" t="s">
+        <v>54</v>
+      </c>
+      <c r="F47" t="s">
+        <v>52</v>
+      </c>
+      <c r="G47" t="s">
+        <v>78</v>
+      </c>
+      <c r="H47" t="s">
+        <v>95</v>
+      </c>
+      <c r="I47" t="s">
+        <v>106</v>
+      </c>
+      <c r="J47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C48" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E48" t="s">
+        <v>55</v>
+      </c>
+      <c r="F48" t="s">
+        <v>52</v>
+      </c>
+      <c r="G48" t="s">
+        <v>78</v>
+      </c>
+      <c r="H48" t="s">
+        <v>95</v>
+      </c>
+      <c r="I48" t="s">
+        <v>107</v>
+      </c>
+      <c r="J48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" t="s">
         <v>50</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C49" t="s">
         <v>47</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E49" t="s">
         <v>62</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F49" t="s">
         <v>62</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G49" t="s">
         <v>78</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="I49" s="2" t="s">
         <v>93</v>
       </c>
     </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E50" t="s">
+        <v>124</v>
+      </c>
+      <c r="F50" t="s">
+        <v>127</v>
+      </c>
+      <c r="G50" t="s">
+        <v>78</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" t="s">
+        <v>120</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E51" t="s">
+        <v>121</v>
+      </c>
+      <c r="F51" t="s">
+        <v>122</v>
+      </c>
+      <c r="G51" t="s">
+        <v>78</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>45</v>
+      </c>
+      <c r="B52" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" t="s">
+        <v>120</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E52" t="s">
+        <v>125</v>
+      </c>
+      <c r="F52" t="s">
+        <v>126</v>
+      </c>
+      <c r="G52" t="s">
+        <v>78</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" t="s">
+        <v>128</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E53" t="s">
+        <v>129</v>
+      </c>
+      <c r="F53" t="s">
+        <v>130</v>
+      </c>
+      <c r="G53" t="s">
+        <v>78</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I40" xr:uid="{A6AE9C97-1A9B-4E5C-B3DE-14E0EEA5BEA2}"/>
+  <autoFilter ref="A1:I53" xr:uid="{A6AE9C97-1A9B-4E5C-B3DE-14E0EEA5BEA2}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add hatchery, update xwalks, fix errors
</commit_message>
<xml_diff>
--- a/example-comp/fish-data-comp-species-fields.xlsx
+++ b/example-comp/fish-data-comp-species-fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edlabola\code\fish-data-comp\example-comp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C1AEA5-712F-4249-90A8-7F6266FE4A6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9BD3925-AEBD-42DE-AD6B-45B6623F0A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58A22057-1635-412A-8133-84FB790BB4D0}"/>
   </bookViews>
@@ -110,9 +110,6 @@
     <t>Integer</t>
   </si>
   <si>
-    <t>For a complete list of SpecieID codes contact the regional StreamNet personnel.</t>
-  </si>
-  <si>
     <t>Partial list: 1 = Chinkook salmon; 2 = Coho salmon; 3 = Steelhead; 4 = Sockeye salmon; 5 = Chum salmon; 6 = Pink salmon; 39 = Mixed salmon; 96 = Mixed anadromous salmonids; 66 = Kokanee; 14 = Bull trout; 10 = Brown trout; 11 = Brook trout; 9 = Rainbow trout; 23 = Redband trout; 111 = Rainbow/redband/steel head trout; 17 = Coastal cutthroat trout; 8 = Cutthroat trout; 94 = Mixed lamprey; 113 = Lamprey (unspecified); 122 = Pacific lamprey; 120 = Western brook lamprey; 15 = Lamprey (CODE DISCONTINUED); 12 = White sturgeon; 44 = Green sturgeon; 98 = N/A; 99 = Unknown</t>
   </si>
   <si>
@@ -441,6 +438,9 @@
   </si>
   <si>
     <t>Enter the name of the run here even if  run name is included in the name of the population. Entries in this field are not recognized as taxonomic divisions</t>
+  </si>
+  <si>
+    <t>Code for the fish species</t>
   </si>
 </sst>
 </file>
@@ -803,9 +803,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AE9C97-1A9B-4E5C-B3DE-14E0EEA5BEA2}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -820,7 +820,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -838,13 +838,13 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" t="s">
         <v>57</v>
       </c>
-      <c r="H1" t="s">
-        <v>58</v>
-      </c>
       <c r="I1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
@@ -864,16 +864,16 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -884,25 +884,25 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="G3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -922,16 +922,16 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -942,25 +942,25 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="G5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -977,19 +977,19 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1006,16 +1006,16 @@
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I7" t="s">
         <v>19</v>
@@ -1029,25 +1029,25 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" t="s">
         <v>112</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>114</v>
       </c>
-      <c r="E8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F8" t="s">
-        <v>115</v>
-      </c>
       <c r="G8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1067,16 +1067,16 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1087,25 +1087,25 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="G10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1122,19 +1122,19 @@
         <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1151,16 +1151,16 @@
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I12" t="s">
         <v>19</v>
@@ -1183,16 +1183,16 @@
         <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1203,25 +1203,25 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D14" t="s">
+        <v>130</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="G14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1238,19 +1238,19 @@
         <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1267,16 +1267,16 @@
         <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I16" t="s">
         <v>19</v>
@@ -1299,16 +1299,16 @@
         <v>8</v>
       </c>
       <c r="F17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1319,25 +1319,25 @@
         <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D18" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1354,19 +1354,19 @@
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1383,16 +1383,16 @@
         <v>18</v>
       </c>
       <c r="E20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I20" t="s">
         <v>19</v>
@@ -1415,16 +1415,16 @@
         <v>8</v>
       </c>
       <c r="F21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1435,25 +1435,25 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D22" t="s">
+        <v>130</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F22" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="G22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1470,19 +1470,19 @@
         <v>18</v>
       </c>
       <c r="E23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1499,16 +1499,16 @@
         <v>18</v>
       </c>
       <c r="E24" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I24" t="s">
         <v>19</v>
@@ -1531,16 +1531,16 @@
         <v>8</v>
       </c>
       <c r="F25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1551,25 +1551,25 @@
         <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D26" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="G26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1586,19 +1586,19 @@
         <v>18</v>
       </c>
       <c r="E27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1615,16 +1615,16 @@
         <v>18</v>
       </c>
       <c r="E28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I28" t="s">
         <v>19</v>
@@ -1638,25 +1638,25 @@
         <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D29" t="s">
         <v>22</v>
       </c>
       <c r="E29" t="s">
+        <v>133</v>
+      </c>
+      <c r="F29" t="s">
         <v>23</v>
       </c>
-      <c r="F29" t="s">
-        <v>24</v>
-      </c>
       <c r="G29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -1667,25 +1667,25 @@
         <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" t="s">
         <v>33</v>
       </c>
-      <c r="F30" t="s">
-        <v>34</v>
-      </c>
       <c r="G30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -1693,28 +1693,28 @@
         <v>20</v>
       </c>
       <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
         <v>25</v>
-      </c>
-      <c r="C31" t="s">
-        <v>26</v>
       </c>
       <c r="D31" t="s">
         <v>22</v>
       </c>
       <c r="E31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -1722,28 +1722,28 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
@@ -1751,28 +1751,28 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I33" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
@@ -1780,28 +1780,28 @@
         <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D34" t="s">
         <v>22</v>
       </c>
       <c r="E34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
@@ -1809,28 +1809,28 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D35" t="s">
+        <v>30</v>
+      </c>
+      <c r="E35" t="s">
         <v>31</v>
       </c>
-      <c r="E35" t="s">
-        <v>32</v>
-      </c>
       <c r="F35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
@@ -1838,28 +1838,28 @@
         <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E36" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" t="s">
         <v>33</v>
       </c>
-      <c r="F36" t="s">
-        <v>34</v>
-      </c>
       <c r="G36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
@@ -1870,498 +1870,498 @@
         <v>21</v>
       </c>
       <c r="C37" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" t="s">
         <v>116</v>
       </c>
-      <c r="D37" t="s">
-        <v>31</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
+        <v>118</v>
+      </c>
+      <c r="G37" t="s">
         <v>117</v>
       </c>
-      <c r="F37" t="s">
-        <v>119</v>
-      </c>
-      <c r="G37" t="s">
-        <v>118</v>
-      </c>
       <c r="H37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
+        <v>74</v>
+      </c>
+      <c r="C38" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" t="s">
         <v>75</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E38" t="s">
         <v>65</v>
       </c>
-      <c r="D38" t="s">
-        <v>76</v>
-      </c>
-      <c r="E38" t="s">
-        <v>66</v>
-      </c>
       <c r="F38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" t="s">
+        <v>76</v>
+      </c>
+      <c r="E39" t="s">
         <v>69</v>
       </c>
-      <c r="D39" t="s">
-        <v>77</v>
-      </c>
-      <c r="E39" t="s">
-        <v>70</v>
-      </c>
       <c r="F39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I39" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G40" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" t="s">
         <v>37</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>38</v>
       </c>
-      <c r="C41" t="s">
-        <v>39</v>
-      </c>
       <c r="D41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F41" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I41" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I42" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I43" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E44" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I44" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>46</v>
       </c>
-      <c r="C46" t="s">
-        <v>47</v>
-      </c>
       <c r="D46" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E46" t="s">
+        <v>50</v>
+      </c>
+      <c r="F46" t="s">
+        <v>51</v>
+      </c>
+      <c r="G46" t="s">
         <v>77</v>
       </c>
-      <c r="E46" t="s">
-        <v>51</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="H46" t="s">
+        <v>94</v>
+      </c>
+      <c r="I46" t="s">
         <v>52</v>
       </c>
-      <c r="G46" t="s">
-        <v>78</v>
-      </c>
-      <c r="H46" t="s">
-        <v>95</v>
-      </c>
-      <c r="I46" t="s">
-        <v>53</v>
-      </c>
       <c r="J46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C47" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D47" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F47" t="s">
+        <v>51</v>
+      </c>
+      <c r="G47" t="s">
         <v>77</v>
       </c>
-      <c r="E47" t="s">
-        <v>54</v>
-      </c>
-      <c r="F47" t="s">
-        <v>52</v>
-      </c>
-      <c r="G47" t="s">
-        <v>78</v>
-      </c>
       <c r="H47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I47" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E48" t="s">
+        <v>54</v>
+      </c>
+      <c r="F48" t="s">
+        <v>51</v>
+      </c>
+      <c r="G48" t="s">
         <v>77</v>
       </c>
-      <c r="E48" t="s">
+      <c r="H48" t="s">
+        <v>94</v>
+      </c>
+      <c r="I48" t="s">
+        <v>106</v>
+      </c>
+      <c r="J48" t="s">
         <v>55</v>
-      </c>
-      <c r="F48" t="s">
-        <v>52</v>
-      </c>
-      <c r="G48" t="s">
-        <v>78</v>
-      </c>
-      <c r="H48" t="s">
-        <v>95</v>
-      </c>
-      <c r="I48" t="s">
-        <v>107</v>
-      </c>
-      <c r="J48" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E49" t="s">
         <v>61</v>
       </c>
-      <c r="E49" t="s">
-        <v>62</v>
-      </c>
       <c r="F49" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I49" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" t="s">
         <v>45</v>
       </c>
-      <c r="B50" t="s">
-        <v>46</v>
-      </c>
       <c r="C50" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E50" t="s">
         <v>123</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="F50" t="s">
+        <v>126</v>
+      </c>
+      <c r="G50" t="s">
         <v>77</v>
       </c>
-      <c r="E50" t="s">
-        <v>124</v>
-      </c>
-      <c r="F50" t="s">
-        <v>127</v>
-      </c>
-      <c r="G50" t="s">
-        <v>78</v>
-      </c>
       <c r="H50" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C51" t="s">
+        <v>119</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E51" t="s">
         <v>120</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="F51" t="s">
+        <v>121</v>
+      </c>
+      <c r="G51" t="s">
         <v>77</v>
       </c>
-      <c r="E51" t="s">
-        <v>121</v>
-      </c>
-      <c r="F51" t="s">
-        <v>122</v>
-      </c>
-      <c r="G51" t="s">
-        <v>78</v>
-      </c>
       <c r="H51" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E52" t="s">
+        <v>124</v>
+      </c>
+      <c r="F52" t="s">
+        <v>125</v>
+      </c>
+      <c r="G52" t="s">
         <v>77</v>
       </c>
-      <c r="E52" t="s">
-        <v>125</v>
-      </c>
-      <c r="F52" t="s">
-        <v>126</v>
-      </c>
-      <c r="G52" t="s">
-        <v>78</v>
-      </c>
       <c r="H52" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>44</v>
+      </c>
+      <c r="B53" t="s">
         <v>45</v>
       </c>
-      <c r="B53" t="s">
-        <v>46</v>
-      </c>
       <c r="C53" t="s">
+        <v>127</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E53" t="s">
         <v>128</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E53" t="s">
+      <c r="F53" t="s">
         <v>129</v>
       </c>
-      <c r="F53" t="s">
-        <v>130</v>
-      </c>
       <c r="G53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>